<commit_message>
Add zopper order id in sheet and make input field to decimal
</commit_message>
<xml_diff>
--- a/application/controllers/excel-templates/Estimate_Sheet.xlsx
+++ b/application/controllers/excel-templates/Estimate_Sheet.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="42">
   <si>
     <t>Blackmelon Advance Technology Co. Pvt. Ltd.</t>
   </si>
@@ -41,6 +41,9 @@
   </si>
   <si>
     <t>Date: {estimate:date}</t>
+  </si>
+  <si>
+    <t>Zopper Order ID: {estimate:order_id}</t>
   </si>
   <si>
     <t>Customer Name</t>
@@ -244,7 +247,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="51">
+  <borders count="48">
     <border/>
     <border>
       <left style="medium">
@@ -653,26 +656,11 @@
         <color rgb="FF000000"/>
       </bottom>
     </border>
-    <border>
-      <left style="medium">
-        <color rgb="FF000000"/>
-      </left>
-      <bottom/>
-    </border>
-    <border>
-      <bottom/>
-    </border>
-    <border>
-      <right style="medium">
-        <color rgb="FF000000"/>
-      </right>
-      <bottom/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="90">
+  <cellXfs count="88">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -755,14 +743,17 @@
     <xf borderId="21" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="22" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="17" fillId="0" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0" vertical="center"/>
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf borderId="23" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="24" fillId="0" fontId="11" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0"/>
+      <alignment horizontal="left"/>
     </xf>
     <xf borderId="24" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="25" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="17" fillId="0" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0" vertical="center"/>
+    </xf>
     <xf borderId="1" fillId="2" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
@@ -774,10 +765,10 @@
     <xf borderId="27" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="28" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="9" fillId="0" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
+      <alignment shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
     <xf borderId="6" fillId="0" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
+      <alignment shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
     <xf borderId="29" fillId="3" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
       <alignment horizontal="left"/>
@@ -805,17 +796,17 @@
     </xf>
     <xf borderId="36" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="4" fillId="0" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
+      <alignment horizontal="left" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
     <xf borderId="37" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="38" fillId="0" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" vertical="center"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf borderId="39" fillId="0" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" vertical="center"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf borderId="9" fillId="2" fontId="12" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" vertical="center"/>
@@ -825,7 +816,7 @@
       <alignment vertical="center"/>
     </xf>
     <xf borderId="10" fillId="0" fontId="13" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" vertical="center"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf borderId="42" fillId="0" fontId="13" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" vertical="center"/>
@@ -837,28 +828,28 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf borderId="20" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" vertical="center"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf borderId="1" fillId="0" fontId="13" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
+      <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
     <xf borderId="43" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf borderId="44" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="43" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" vertical="center"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf borderId="45" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf borderId="46" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="45" fillId="0" fontId="6" numFmtId="1" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="center" readingOrder="0" vertical="center"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf borderId="47" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="1" fillId="3" fontId="13" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0" vertical="top"/>
+      <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf borderId="1" fillId="0" fontId="13" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" vertical="center"/>
@@ -869,9 +860,6 @@
     <xf borderId="9" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf borderId="48" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="49" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="50" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="0" fillId="0" fontId="15" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -900,7 +888,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image2.png"/>
+        <xdr:cNvPr id="0" name="image1.png"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -925,18 +913,18 @@
     <xdr:from>
       <xdr:col>7</xdr:col>
       <xdr:colOff>66675</xdr:colOff>
-      <xdr:row>20</xdr:row>
+      <xdr:row>21</xdr:row>
       <xdr:rowOff>19050</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
       <xdr:colOff>266700</xdr:colOff>
-      <xdr:row>27</xdr:row>
+      <xdr:row>28</xdr:row>
       <xdr:rowOff>104775</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image1.jpg" title="Image"/>
+        <xdr:cNvPr id="0" name="image3.jpg" title="Image"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -961,18 +949,18 @@
     <xdr:from>
       <xdr:col>11</xdr:col>
       <xdr:colOff>47625</xdr:colOff>
-      <xdr:row>23</xdr:row>
+      <xdr:row>24</xdr:row>
       <xdr:rowOff>9525</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
       <xdr:colOff>19050</xdr:colOff>
-      <xdr:row>24</xdr:row>
+      <xdr:row>25</xdr:row>
       <xdr:rowOff>152400</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image3.png" title="Image"/>
+        <xdr:cNvPr id="0" name="image2.png" title="Image"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -1224,308 +1212,313 @@
       <c r="Q10" s="41"/>
       <c r="R10" s="1"/>
     </row>
-    <row r="11" ht="15.0" customHeight="1">
+    <row r="11">
       <c r="A11" s="1"/>
       <c r="B11" s="42" t="s">
         <v>10</v>
       </c>
-      <c r="C11" s="3"/>
-      <c r="D11" s="3"/>
-      <c r="E11" s="3"/>
-      <c r="F11" s="3"/>
-      <c r="G11" s="4"/>
-      <c r="H11" s="43" t="s">
-        <v>11</v>
-      </c>
-      <c r="I11" s="38"/>
-      <c r="J11" s="43" t="s">
-        <v>12</v>
-      </c>
-      <c r="K11" s="32"/>
-      <c r="L11" s="32"/>
-      <c r="M11" s="38"/>
-      <c r="N11" s="43" t="s">
-        <v>13</v>
-      </c>
-      <c r="O11" s="32"/>
-      <c r="P11" s="32"/>
-      <c r="Q11" s="33"/>
+      <c r="C11" s="32"/>
+      <c r="D11" s="32"/>
+      <c r="E11" s="32"/>
+      <c r="F11" s="32"/>
+      <c r="G11" s="32"/>
+      <c r="H11" s="32"/>
+      <c r="I11" s="32"/>
+      <c r="J11" s="32"/>
+      <c r="K11" s="38"/>
+      <c r="L11" s="39"/>
+      <c r="M11" s="40"/>
+      <c r="N11" s="40"/>
+      <c r="O11" s="40"/>
+      <c r="P11" s="40"/>
+      <c r="Q11" s="41"/>
       <c r="R11" s="1"/>
     </row>
     <row r="12" ht="15.0" customHeight="1">
       <c r="A12" s="1"/>
-      <c r="B12" s="44"/>
-      <c r="C12" s="19"/>
-      <c r="D12" s="19"/>
-      <c r="E12" s="19"/>
-      <c r="F12" s="19"/>
-      <c r="G12" s="45"/>
-      <c r="H12" s="46"/>
-      <c r="I12" s="47"/>
-      <c r="J12" s="46"/>
-      <c r="K12" s="35"/>
-      <c r="L12" s="35"/>
-      <c r="M12" s="47"/>
-      <c r="N12" s="46"/>
-      <c r="O12" s="35"/>
-      <c r="P12" s="35"/>
-      <c r="Q12" s="36"/>
+      <c r="B12" s="43" t="s">
+        <v>11</v>
+      </c>
+      <c r="C12" s="3"/>
+      <c r="D12" s="3"/>
+      <c r="E12" s="3"/>
+      <c r="F12" s="3"/>
+      <c r="G12" s="4"/>
+      <c r="H12" s="44" t="s">
+        <v>12</v>
+      </c>
+      <c r="I12" s="38"/>
+      <c r="J12" s="44" t="s">
+        <v>13</v>
+      </c>
+      <c r="K12" s="32"/>
+      <c r="L12" s="32"/>
+      <c r="M12" s="38"/>
+      <c r="N12" s="44" t="s">
+        <v>14</v>
+      </c>
+      <c r="O12" s="32"/>
+      <c r="P12" s="32"/>
+      <c r="Q12" s="33"/>
       <c r="R12" s="1"/>
     </row>
     <row r="13" ht="15.0" customHeight="1">
       <c r="A13" s="1"/>
-      <c r="B13" s="48" t="s">
-        <v>14</v>
-      </c>
-      <c r="C13" s="24"/>
-      <c r="D13" s="24"/>
-      <c r="E13" s="24"/>
-      <c r="F13" s="24"/>
-      <c r="G13" s="25"/>
-      <c r="H13" s="49" t="s">
-        <v>15</v>
-      </c>
-      <c r="I13" s="45"/>
-      <c r="J13" s="49" t="s">
-        <v>16</v>
-      </c>
-      <c r="K13" s="19"/>
-      <c r="L13" s="19"/>
-      <c r="M13" s="45"/>
-      <c r="N13" s="49" t="s">
-        <v>17</v>
-      </c>
-      <c r="O13" s="19"/>
-      <c r="P13" s="19"/>
-      <c r="Q13" s="45"/>
-      <c r="R13" s="50"/>
+      <c r="B13" s="45"/>
+      <c r="C13" s="19"/>
+      <c r="D13" s="19"/>
+      <c r="E13" s="19"/>
+      <c r="F13" s="19"/>
+      <c r="G13" s="46"/>
+      <c r="H13" s="47"/>
+      <c r="I13" s="48"/>
+      <c r="J13" s="47"/>
+      <c r="K13" s="35"/>
+      <c r="L13" s="35"/>
+      <c r="M13" s="48"/>
+      <c r="N13" s="47"/>
+      <c r="O13" s="35"/>
+      <c r="P13" s="35"/>
+      <c r="Q13" s="36"/>
+      <c r="R13" s="1"/>
     </row>
     <row r="14" ht="15.0" customHeight="1">
       <c r="A14" s="1"/>
-      <c r="B14" s="51" t="s">
+      <c r="B14" s="49" t="s">
+        <v>15</v>
+      </c>
+      <c r="C14" s="24"/>
+      <c r="D14" s="24"/>
+      <c r="E14" s="24"/>
+      <c r="F14" s="24"/>
+      <c r="G14" s="25"/>
+      <c r="H14" s="50" t="s">
+        <v>16</v>
+      </c>
+      <c r="I14" s="46"/>
+      <c r="J14" s="50" t="s">
+        <v>17</v>
+      </c>
+      <c r="K14" s="19"/>
+      <c r="L14" s="19"/>
+      <c r="M14" s="46"/>
+      <c r="N14" s="50" t="s">
         <v>18</v>
       </c>
-      <c r="C14" s="3"/>
-      <c r="D14" s="3"/>
-      <c r="E14" s="3"/>
-      <c r="F14" s="3"/>
-      <c r="G14" s="52"/>
-      <c r="H14" s="51" t="s">
+      <c r="O14" s="19"/>
+      <c r="P14" s="19"/>
+      <c r="Q14" s="46"/>
+      <c r="R14" s="51"/>
+    </row>
+    <row r="15" ht="15.0" customHeight="1">
+      <c r="A15" s="1"/>
+      <c r="B15" s="52" t="s">
         <v>19</v>
       </c>
-      <c r="I14" s="3"/>
-      <c r="J14" s="52"/>
-      <c r="K14" s="53" t="s">
+      <c r="C15" s="3"/>
+      <c r="D15" s="3"/>
+      <c r="E15" s="3"/>
+      <c r="F15" s="3"/>
+      <c r="G15" s="53"/>
+      <c r="H15" s="52" t="s">
         <v>20</v>
       </c>
-      <c r="L14" s="52"/>
-      <c r="M14" s="54" t="s">
+      <c r="I15" s="3"/>
+      <c r="J15" s="53"/>
+      <c r="K15" s="54" t="s">
         <v>21</v>
       </c>
-      <c r="N14" s="27"/>
-      <c r="O14" s="28"/>
-      <c r="P14" s="55" t="s">
+      <c r="L15" s="53"/>
+      <c r="M15" s="55" t="s">
         <v>22</v>
       </c>
-      <c r="Q14" s="4"/>
-      <c r="R14" s="1"/>
-    </row>
-    <row r="15">
-      <c r="A15" s="1"/>
-      <c r="B15" s="44"/>
-      <c r="C15" s="19"/>
-      <c r="D15" s="19"/>
-      <c r="E15" s="19"/>
-      <c r="F15" s="19"/>
-      <c r="G15" s="56"/>
-      <c r="H15" s="44"/>
-      <c r="I15" s="19"/>
-      <c r="J15" s="56"/>
-      <c r="K15" s="57"/>
-      <c r="L15" s="56"/>
-      <c r="M15" s="58" t="s">
+      <c r="N15" s="27"/>
+      <c r="O15" s="28"/>
+      <c r="P15" s="56" t="s">
         <v>23</v>
       </c>
-      <c r="N15" s="59" t="s">
+      <c r="Q15" s="4"/>
+      <c r="R15" s="1"/>
+    </row>
+    <row r="16">
+      <c r="A16" s="1"/>
+      <c r="B16" s="45"/>
+      <c r="C16" s="19"/>
+      <c r="D16" s="19"/>
+      <c r="E16" s="19"/>
+      <c r="F16" s="19"/>
+      <c r="G16" s="57"/>
+      <c r="H16" s="45"/>
+      <c r="I16" s="19"/>
+      <c r="J16" s="57"/>
+      <c r="K16" s="58"/>
+      <c r="L16" s="57"/>
+      <c r="M16" s="59" t="s">
         <v>24</v>
       </c>
-      <c r="O15" s="60"/>
-      <c r="P15" s="57"/>
-      <c r="Q15" s="45"/>
-      <c r="R15" s="1"/>
-    </row>
-    <row r="16" ht="28.5" customHeight="1">
-      <c r="A16" s="1"/>
-      <c r="B16" s="61" t="s">
+      <c r="N16" s="60" t="s">
         <v>25</v>
       </c>
-      <c r="G16" s="62"/>
-      <c r="H16" s="63" t="s">
+      <c r="O16" s="61"/>
+      <c r="P16" s="58"/>
+      <c r="Q16" s="46"/>
+      <c r="R16" s="1"/>
+    </row>
+    <row r="17" ht="28.5" customHeight="1">
+      <c r="A17" s="1"/>
+      <c r="B17" s="62" t="s">
         <v>26</v>
       </c>
-      <c r="J16" s="62"/>
-      <c r="K16" s="64" t="s">
+      <c r="G17" s="63"/>
+      <c r="H17" s="64" t="s">
         <v>27</v>
       </c>
-      <c r="L16" s="62"/>
-      <c r="M16" s="65" t="s">
+      <c r="J17" s="63"/>
+      <c r="K17" s="65" t="s">
         <v>28</v>
       </c>
-      <c r="N16" s="64" t="s">
+      <c r="L17" s="63"/>
+      <c r="M17" s="66" t="s">
         <v>29</v>
       </c>
-      <c r="O16" s="62"/>
-      <c r="P16" s="64" t="s">
+      <c r="N17" s="65" t="s">
         <v>30</v>
       </c>
-      <c r="Q16" s="9"/>
-      <c r="R16" s="1"/>
-    </row>
-    <row r="17" ht="18.75" customHeight="1">
-      <c r="A17" s="1"/>
-      <c r="B17" s="66" t="s">
-        <v>22</v>
-      </c>
-      <c r="C17" s="24"/>
-      <c r="D17" s="24"/>
-      <c r="E17" s="24"/>
-      <c r="F17" s="24"/>
-      <c r="G17" s="67"/>
-      <c r="H17" s="68"/>
-      <c r="I17" s="24"/>
-      <c r="J17" s="67"/>
-      <c r="K17" s="69" t="s">
-        <v>27</v>
-      </c>
-      <c r="L17" s="67"/>
-      <c r="M17" s="70"/>
-      <c r="N17" s="69" t="s">
-        <v>29</v>
-      </c>
-      <c r="O17" s="67"/>
-      <c r="P17" s="69" t="s">
+      <c r="O17" s="63"/>
+      <c r="P17" s="65" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q17" s="9"/>
+      <c r="R17" s="1"/>
+    </row>
+    <row r="18" ht="18.75" customHeight="1">
+      <c r="A18" s="1"/>
+      <c r="B18" s="67" t="s">
+        <v>23</v>
+      </c>
+      <c r="C18" s="24"/>
+      <c r="D18" s="24"/>
+      <c r="E18" s="24"/>
+      <c r="F18" s="24"/>
+      <c r="G18" s="68"/>
+      <c r="H18" s="69"/>
+      <c r="I18" s="24"/>
+      <c r="J18" s="68"/>
+      <c r="K18" s="70" t="s">
+        <v>28</v>
+      </c>
+      <c r="L18" s="68"/>
+      <c r="M18" s="71"/>
+      <c r="N18" s="70" t="s">
         <v>30</v>
       </c>
-      <c r="Q17" s="25"/>
-      <c r="R17" s="1"/>
-    </row>
-    <row r="18">
-      <c r="A18" s="1"/>
-      <c r="B18" s="71" t="s">
+      <c r="O18" s="68"/>
+      <c r="P18" s="70" t="s">
         <v>31</v>
       </c>
-      <c r="C18" s="19"/>
-      <c r="D18" s="19"/>
-      <c r="E18" s="19"/>
-      <c r="F18" s="19"/>
-      <c r="G18" s="19"/>
-      <c r="H18" s="19"/>
-      <c r="I18" s="19"/>
-      <c r="J18" s="19"/>
-      <c r="K18" s="72" t="s">
-        <v>32</v>
-      </c>
-      <c r="L18" s="35"/>
-      <c r="M18" s="35"/>
-      <c r="N18" s="35"/>
-      <c r="O18" s="47"/>
-      <c r="P18" s="73" t="s">
-        <v>27</v>
-      </c>
-      <c r="Q18" s="36"/>
+      <c r="Q18" s="25"/>
       <c r="R18" s="1"/>
     </row>
     <row r="19">
       <c r="A19" s="1"/>
-      <c r="B19" s="74" t="s">
+      <c r="B19" s="72" t="s">
+        <v>32</v>
+      </c>
+      <c r="C19" s="19"/>
+      <c r="D19" s="19"/>
+      <c r="E19" s="19"/>
+      <c r="F19" s="19"/>
+      <c r="G19" s="19"/>
+      <c r="H19" s="19"/>
+      <c r="I19" s="19"/>
+      <c r="J19" s="19"/>
+      <c r="K19" s="73" t="s">
         <v>33</v>
       </c>
-      <c r="C19" s="3"/>
-      <c r="D19" s="3"/>
-      <c r="E19" s="3"/>
-      <c r="F19" s="3"/>
-      <c r="G19" s="3"/>
-      <c r="H19" s="3"/>
-      <c r="I19" s="3"/>
-      <c r="J19" s="4"/>
-      <c r="K19" s="75" t="s">
-        <v>34</v>
-      </c>
-      <c r="L19" s="40"/>
-      <c r="M19" s="40"/>
-      <c r="N19" s="40"/>
-      <c r="O19" s="76"/>
-      <c r="P19" s="77" t="s">
-        <v>29</v>
-      </c>
-      <c r="Q19" s="41"/>
+      <c r="L19" s="35"/>
+      <c r="M19" s="35"/>
+      <c r="N19" s="35"/>
+      <c r="O19" s="48"/>
+      <c r="P19" s="74" t="s">
+        <v>28</v>
+      </c>
+      <c r="Q19" s="36"/>
       <c r="R19" s="1"/>
     </row>
     <row r="20">
       <c r="A20" s="1"/>
-      <c r="B20" s="44"/>
-      <c r="C20" s="19"/>
-      <c r="D20" s="19"/>
-      <c r="E20" s="19"/>
-      <c r="F20" s="19"/>
-      <c r="G20" s="19"/>
-      <c r="H20" s="19"/>
-      <c r="I20" s="19"/>
-      <c r="J20" s="45"/>
-      <c r="K20" s="78" t="s">
+      <c r="B20" s="75" t="s">
+        <v>34</v>
+      </c>
+      <c r="C20" s="3"/>
+      <c r="D20" s="3"/>
+      <c r="E20" s="3"/>
+      <c r="F20" s="3"/>
+      <c r="G20" s="3"/>
+      <c r="H20" s="3"/>
+      <c r="I20" s="3"/>
+      <c r="J20" s="4"/>
+      <c r="K20" s="76" t="s">
         <v>35</v>
       </c>
-      <c r="L20" s="79"/>
-      <c r="M20" s="79"/>
-      <c r="N20" s="79"/>
-      <c r="O20" s="60"/>
-      <c r="P20" s="80" t="s">
+      <c r="L20" s="40"/>
+      <c r="M20" s="40"/>
+      <c r="N20" s="40"/>
+      <c r="O20" s="77"/>
+      <c r="P20" s="78" t="s">
         <v>30</v>
       </c>
-      <c r="Q20" s="81"/>
+      <c r="Q20" s="41"/>
       <c r="R20" s="1"/>
     </row>
     <row r="21">
       <c r="A21" s="1"/>
-      <c r="B21" s="82" t="s">
+      <c r="B21" s="45"/>
+      <c r="C21" s="19"/>
+      <c r="D21" s="19"/>
+      <c r="E21" s="19"/>
+      <c r="F21" s="19"/>
+      <c r="G21" s="19"/>
+      <c r="H21" s="19"/>
+      <c r="I21" s="19"/>
+      <c r="J21" s="46"/>
+      <c r="K21" s="79" t="s">
         <v>36</v>
       </c>
-      <c r="C21" s="3"/>
-      <c r="D21" s="3"/>
-      <c r="E21" s="3"/>
-      <c r="F21" s="3"/>
-      <c r="G21" s="4"/>
-      <c r="H21" s="83"/>
-      <c r="I21" s="3"/>
-      <c r="J21" s="4"/>
-      <c r="K21" s="84" t="s">
-        <v>37</v>
-      </c>
-      <c r="L21" s="24"/>
-      <c r="M21" s="24"/>
-      <c r="N21" s="24"/>
-      <c r="O21" s="25"/>
-      <c r="P21" s="85">
-        <v>0.0</v>
-      </c>
-      <c r="Q21" s="25"/>
+      <c r="L21" s="80"/>
+      <c r="M21" s="80"/>
+      <c r="N21" s="80"/>
+      <c r="O21" s="61"/>
+      <c r="P21" s="81" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q21" s="82"/>
       <c r="R21" s="1"/>
     </row>
     <row r="22">
       <c r="A22" s="1"/>
-      <c r="B22" s="10"/>
-      <c r="G22" s="9"/>
-      <c r="H22" s="10"/>
-      <c r="J22" s="9"/>
-      <c r="K22" s="51" t="s">
+      <c r="B22" s="83" t="s">
+        <v>37</v>
+      </c>
+      <c r="C22" s="3"/>
+      <c r="D22" s="3"/>
+      <c r="E22" s="3"/>
+      <c r="F22" s="3"/>
+      <c r="G22" s="4"/>
+      <c r="H22" s="84"/>
+      <c r="I22" s="3"/>
+      <c r="J22" s="4"/>
+      <c r="K22" s="85" t="s">
         <v>38</v>
       </c>
-      <c r="L22" s="3"/>
-      <c r="M22" s="3"/>
-      <c r="N22" s="3"/>
-      <c r="O22" s="3"/>
-      <c r="P22" s="3"/>
-      <c r="Q22" s="4"/>
+      <c r="L22" s="24"/>
+      <c r="M22" s="24"/>
+      <c r="N22" s="24"/>
+      <c r="O22" s="25"/>
+      <c r="P22" s="86">
+        <v>0.0</v>
+      </c>
+      <c r="Q22" s="25"/>
       <c r="R22" s="1"/>
     </row>
     <row r="23">
@@ -1534,13 +1527,15 @@
       <c r="G23" s="9"/>
       <c r="H23" s="10"/>
       <c r="J23" s="9"/>
-      <c r="K23" s="86"/>
-      <c r="L23" s="87"/>
-      <c r="M23" s="87"/>
-      <c r="N23" s="87"/>
-      <c r="O23" s="87"/>
-      <c r="P23" s="87"/>
-      <c r="Q23" s="88"/>
+      <c r="K23" s="52" t="s">
+        <v>39</v>
+      </c>
+      <c r="L23" s="3"/>
+      <c r="M23" s="3"/>
+      <c r="N23" s="3"/>
+      <c r="O23" s="3"/>
+      <c r="P23" s="3"/>
+      <c r="Q23" s="4"/>
       <c r="R23" s="1"/>
     </row>
     <row r="24">
@@ -1549,13 +1544,8 @@
       <c r="G24" s="9"/>
       <c r="H24" s="10"/>
       <c r="J24" s="9"/>
-      <c r="K24" s="83"/>
-      <c r="L24" s="3"/>
-      <c r="M24" s="3"/>
-      <c r="N24" s="3"/>
-      <c r="O24" s="3"/>
-      <c r="P24" s="3"/>
-      <c r="Q24" s="4"/>
+      <c r="K24" s="10"/>
+      <c r="Q24" s="9"/>
       <c r="R24" s="1"/>
     </row>
     <row r="25">
@@ -1564,11 +1554,16 @@
       <c r="G25" s="9"/>
       <c r="H25" s="10"/>
       <c r="J25" s="9"/>
-      <c r="K25" s="10"/>
-      <c r="Q25" s="9"/>
+      <c r="K25" s="84"/>
+      <c r="L25" s="3"/>
+      <c r="M25" s="3"/>
+      <c r="N25" s="3"/>
+      <c r="O25" s="3"/>
+      <c r="P25" s="3"/>
+      <c r="Q25" s="4"/>
       <c r="R25" s="1"/>
     </row>
-    <row r="26" ht="3.75" hidden="1" customHeight="1">
+    <row r="26">
       <c r="A26" s="1"/>
       <c r="B26" s="10"/>
       <c r="G26" s="9"/>
@@ -1578,122 +1573,134 @@
       <c r="Q26" s="9"/>
       <c r="R26" s="1"/>
     </row>
-    <row r="27" ht="0.75" customHeight="1">
+    <row r="27" ht="3.75" hidden="1" customHeight="1">
       <c r="A27" s="1"/>
       <c r="B27" s="10"/>
       <c r="G27" s="9"/>
       <c r="H27" s="10"/>
       <c r="J27" s="9"/>
-      <c r="K27" s="44"/>
-      <c r="L27" s="19"/>
-      <c r="M27" s="19"/>
-      <c r="N27" s="19"/>
-      <c r="O27" s="19"/>
-      <c r="P27" s="19"/>
-      <c r="Q27" s="45"/>
+      <c r="K27" s="10"/>
+      <c r="Q27" s="9"/>
       <c r="R27" s="1"/>
     </row>
-    <row r="28">
+    <row r="28" ht="0.75" customHeight="1">
       <c r="A28" s="1"/>
-      <c r="B28" s="44"/>
-      <c r="C28" s="19"/>
-      <c r="D28" s="19"/>
-      <c r="E28" s="19"/>
-      <c r="F28" s="19"/>
-      <c r="G28" s="45"/>
-      <c r="H28" s="44"/>
-      <c r="I28" s="19"/>
-      <c r="J28" s="45"/>
-      <c r="K28" s="71" t="s">
-        <v>39</v>
-      </c>
+      <c r="B28" s="10"/>
+      <c r="G28" s="9"/>
+      <c r="H28" s="10"/>
+      <c r="J28" s="9"/>
+      <c r="K28" s="45"/>
       <c r="L28" s="19"/>
       <c r="M28" s="19"/>
       <c r="N28" s="19"/>
       <c r="O28" s="19"/>
       <c r="P28" s="19"/>
-      <c r="Q28" s="45"/>
+      <c r="Q28" s="46"/>
       <c r="R28" s="1"/>
     </row>
-    <row r="29" ht="3.75" customHeight="1">
+    <row r="29">
       <c r="A29" s="1"/>
-      <c r="B29" s="1"/>
-      <c r="C29" s="1"/>
-      <c r="D29" s="1"/>
-      <c r="E29" s="1"/>
-      <c r="F29" s="1"/>
-      <c r="G29" s="1"/>
-      <c r="H29" s="1"/>
-      <c r="I29" s="1"/>
-      <c r="J29" s="1"/>
-      <c r="K29" s="1"/>
-      <c r="L29" s="1"/>
-      <c r="M29" s="1"/>
-      <c r="N29" s="1"/>
-      <c r="O29" s="1"/>
-      <c r="P29" s="1"/>
-      <c r="Q29" s="1"/>
+      <c r="B29" s="45"/>
+      <c r="C29" s="19"/>
+      <c r="D29" s="19"/>
+      <c r="E29" s="19"/>
+      <c r="F29" s="19"/>
+      <c r="G29" s="46"/>
+      <c r="H29" s="45"/>
+      <c r="I29" s="19"/>
+      <c r="J29" s="46"/>
+      <c r="K29" s="72" t="s">
+        <v>40</v>
+      </c>
+      <c r="L29" s="19"/>
+      <c r="M29" s="19"/>
+      <c r="N29" s="19"/>
+      <c r="O29" s="19"/>
+      <c r="P29" s="19"/>
+      <c r="Q29" s="46"/>
       <c r="R29" s="1"/>
     </row>
-    <row r="30" ht="15.0" customHeight="1">
-      <c r="B30" s="89" t="s">
-        <v>40</v>
+    <row r="30" ht="3.75" customHeight="1">
+      <c r="A30" s="1"/>
+      <c r="B30" s="1"/>
+      <c r="C30" s="1"/>
+      <c r="D30" s="1"/>
+      <c r="E30" s="1"/>
+      <c r="F30" s="1"/>
+      <c r="G30" s="1"/>
+      <c r="H30" s="1"/>
+      <c r="I30" s="1"/>
+      <c r="J30" s="1"/>
+      <c r="K30" s="1"/>
+      <c r="L30" s="1"/>
+      <c r="M30" s="1"/>
+      <c r="N30" s="1"/>
+      <c r="O30" s="1"/>
+      <c r="P30" s="1"/>
+      <c r="Q30" s="1"/>
+      <c r="R30" s="1"/>
+    </row>
+    <row r="31" ht="15.0" customHeight="1">
+      <c r="B31" s="87" t="s">
+        <v>41</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="52">
-    <mergeCell ref="G4:M4"/>
+  <mergeCells count="54">
     <mergeCell ref="F3:N3"/>
+    <mergeCell ref="O3:Q4"/>
+    <mergeCell ref="B8:Q9"/>
+    <mergeCell ref="B10:K10"/>
+    <mergeCell ref="L10:Q10"/>
+    <mergeCell ref="B11:K11"/>
+    <mergeCell ref="L11:Q11"/>
+    <mergeCell ref="H14:I14"/>
+    <mergeCell ref="J14:M14"/>
+    <mergeCell ref="B2:Q2"/>
     <mergeCell ref="L7:Q7"/>
     <mergeCell ref="B7:K7"/>
     <mergeCell ref="B6:Q6"/>
+    <mergeCell ref="B3:C4"/>
+    <mergeCell ref="K21:O21"/>
+    <mergeCell ref="K20:O20"/>
+    <mergeCell ref="N18:O18"/>
+    <mergeCell ref="N17:O17"/>
+    <mergeCell ref="K19:O19"/>
+    <mergeCell ref="K29:Q29"/>
+    <mergeCell ref="K25:Q28"/>
+    <mergeCell ref="K22:O22"/>
+    <mergeCell ref="K23:Q24"/>
+    <mergeCell ref="K17:L17"/>
+    <mergeCell ref="K15:L16"/>
+    <mergeCell ref="B12:G13"/>
+    <mergeCell ref="H12:I13"/>
+    <mergeCell ref="J12:M13"/>
+    <mergeCell ref="N14:Q14"/>
+    <mergeCell ref="N12:Q13"/>
+    <mergeCell ref="P20:Q20"/>
+    <mergeCell ref="P19:Q19"/>
+    <mergeCell ref="P18:Q18"/>
+    <mergeCell ref="P21:Q21"/>
+    <mergeCell ref="P22:Q22"/>
+    <mergeCell ref="P17:Q17"/>
+    <mergeCell ref="B17:G17"/>
+    <mergeCell ref="H17:J17"/>
+    <mergeCell ref="G4:M4"/>
     <mergeCell ref="G5:M5"/>
-    <mergeCell ref="B3:C4"/>
-    <mergeCell ref="O3:Q4"/>
-    <mergeCell ref="B2:Q2"/>
-    <mergeCell ref="P17:Q17"/>
-    <mergeCell ref="P16:Q16"/>
-    <mergeCell ref="P20:Q20"/>
-    <mergeCell ref="P21:Q21"/>
-    <mergeCell ref="P14:Q15"/>
-    <mergeCell ref="M14:O14"/>
-    <mergeCell ref="N15:O15"/>
-    <mergeCell ref="N17:O17"/>
+    <mergeCell ref="B18:G18"/>
+    <mergeCell ref="B19:J19"/>
+    <mergeCell ref="H18:J18"/>
+    <mergeCell ref="B20:J21"/>
+    <mergeCell ref="B31:Q31"/>
+    <mergeCell ref="B22:G29"/>
+    <mergeCell ref="H22:J29"/>
+    <mergeCell ref="P15:Q16"/>
+    <mergeCell ref="M15:O15"/>
     <mergeCell ref="N16:O16"/>
-    <mergeCell ref="B16:G16"/>
-    <mergeCell ref="B14:G15"/>
-    <mergeCell ref="J11:M12"/>
-    <mergeCell ref="J13:M13"/>
-    <mergeCell ref="N13:Q13"/>
-    <mergeCell ref="N11:Q12"/>
-    <mergeCell ref="K18:O18"/>
-    <mergeCell ref="B17:G17"/>
-    <mergeCell ref="B18:J18"/>
-    <mergeCell ref="B11:G12"/>
-    <mergeCell ref="B13:G13"/>
-    <mergeCell ref="B8:Q9"/>
-    <mergeCell ref="H16:J16"/>
-    <mergeCell ref="H17:J17"/>
-    <mergeCell ref="K28:Q28"/>
-    <mergeCell ref="K24:Q27"/>
-    <mergeCell ref="K21:O21"/>
-    <mergeCell ref="K22:Q23"/>
-    <mergeCell ref="K19:O19"/>
-    <mergeCell ref="K20:O20"/>
-    <mergeCell ref="P19:Q19"/>
-    <mergeCell ref="B30:Q30"/>
-    <mergeCell ref="P18:Q18"/>
-    <mergeCell ref="B21:G28"/>
-    <mergeCell ref="B19:J20"/>
-    <mergeCell ref="H21:J28"/>
-    <mergeCell ref="B10:K10"/>
-    <mergeCell ref="L10:Q10"/>
-    <mergeCell ref="K17:L17"/>
-    <mergeCell ref="K16:L16"/>
-    <mergeCell ref="K14:L15"/>
-    <mergeCell ref="H14:J15"/>
-    <mergeCell ref="H11:I12"/>
-    <mergeCell ref="H13:I13"/>
+    <mergeCell ref="B14:G14"/>
+    <mergeCell ref="K18:L18"/>
+    <mergeCell ref="H15:J16"/>
+    <mergeCell ref="B15:G16"/>
   </mergeCells>
   <drawing r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Repair bookings estimate for other partners #CRM-192
</commit_message>
<xml_diff>
--- a/application/controllers/excel-templates/Estimate_Sheet.xlsx
+++ b/application/controllers/excel-templates/Estimate_Sheet.xlsx
@@ -28,13 +28,13 @@
     <t>Estimate Sheet</t>
   </si>
   <si>
-    <t>Name: SOLVY TECH SOLUTIONS PVT LTD</t>
+    <t>Name: {estimate:company_name}</t>
   </si>
   <si>
     <t>GSTIN: 09AAPCS1780F1Z0</t>
   </si>
   <si>
-    <t>Address: H-211 Sector-63, Noida, Gautam Buddha Nagar, Pincode -201301, UTTAR PRADESH</t>
+    <t>{estimate:company_address}</t>
   </si>
   <si>
     <t>247around Booking ID: {estimate:booking_id}</t>
@@ -43,7 +43,7 @@
     <t>Date: {estimate:date}</t>
   </si>
   <si>
-    <t>Zopper Order ID: {estimate:order_id}</t>
+    <t>Order ID: {estimate:order_id}</t>
   </si>
   <si>
     <t>Customer Name</t>
@@ -669,7 +669,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="87">
+  <cellXfs count="88">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -735,7 +735,7 @@
     <xf borderId="10" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="11" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="12" fillId="0" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left" vertical="center"/>
+      <alignment horizontal="left" readingOrder="0" vertical="center"/>
     </xf>
     <xf borderId="13" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="14" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
@@ -744,7 +744,7 @@
     </xf>
     <xf borderId="16" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="17" fillId="0" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left" shrinkToFit="0" vertical="center" wrapText="1"/>
+      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
     <xf borderId="18" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="19" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
@@ -760,6 +760,9 @@
     </xf>
     <xf borderId="24" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="25" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="17" fillId="0" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0" vertical="center"/>
+    </xf>
     <xf borderId="1" fillId="2" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
@@ -802,17 +805,17 @@
     </xf>
     <xf borderId="36" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="4" fillId="0" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
+      <alignment horizontal="left" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
     <xf borderId="37" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="38" fillId="0" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" vertical="center"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" vertical="center"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf borderId="39" fillId="0" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" vertical="center"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf borderId="9" fillId="2" fontId="12" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" vertical="center"/>
@@ -878,7 +881,7 @@
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram">
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram">
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>1</xdr:col>
@@ -930,7 +933,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image3.jpg" title="Image"/>
+        <xdr:cNvPr id="0" name="image2.jpg" title="Image"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -966,7 +969,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image2.png" title="Image"/>
+        <xdr:cNvPr id="0" name="image3.png" title="Image"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -1152,7 +1155,7 @@
       <c r="Q7" s="30"/>
       <c r="R7" s="1"/>
     </row>
-    <row r="8" ht="15.0" customHeight="1">
+    <row r="8">
       <c r="A8" s="1"/>
       <c r="B8" s="31" t="s">
         <v>7</v>
@@ -1220,7 +1223,7 @@
     </row>
     <row r="11">
       <c r="A11" s="1"/>
-      <c r="B11" s="37" t="s">
+      <c r="B11" s="42" t="s">
         <v>10</v>
       </c>
       <c r="C11" s="32"/>
@@ -1240,9 +1243,9 @@
       <c r="Q11" s="41"/>
       <c r="R11" s="1"/>
     </row>
-    <row r="12" ht="15.0" customHeight="1">
+    <row r="12">
       <c r="A12" s="1"/>
-      <c r="B12" s="42" t="s">
+      <c r="B12" s="43" t="s">
         <v>11</v>
       </c>
       <c r="C12" s="3"/>
@@ -1250,17 +1253,17 @@
       <c r="E12" s="3"/>
       <c r="F12" s="3"/>
       <c r="G12" s="4"/>
-      <c r="H12" s="43" t="s">
+      <c r="H12" s="44" t="s">
         <v>12</v>
       </c>
       <c r="I12" s="38"/>
-      <c r="J12" s="43" t="s">
+      <c r="J12" s="44" t="s">
         <v>13</v>
       </c>
       <c r="K12" s="32"/>
       <c r="L12" s="32"/>
       <c r="M12" s="38"/>
-      <c r="N12" s="43" t="s">
+      <c r="N12" s="44" t="s">
         <v>14</v>
       </c>
       <c r="O12" s="32"/>
@@ -1268,29 +1271,29 @@
       <c r="Q12" s="33"/>
       <c r="R12" s="1"/>
     </row>
-    <row r="13" ht="15.0" customHeight="1">
+    <row r="13">
       <c r="A13" s="1"/>
-      <c r="B13" s="44"/>
+      <c r="B13" s="45"/>
       <c r="C13" s="19"/>
       <c r="D13" s="19"/>
       <c r="E13" s="19"/>
       <c r="F13" s="19"/>
-      <c r="G13" s="45"/>
-      <c r="H13" s="46"/>
-      <c r="I13" s="47"/>
-      <c r="J13" s="46"/>
+      <c r="G13" s="46"/>
+      <c r="H13" s="47"/>
+      <c r="I13" s="48"/>
+      <c r="J13" s="47"/>
       <c r="K13" s="35"/>
       <c r="L13" s="35"/>
-      <c r="M13" s="47"/>
-      <c r="N13" s="46"/>
+      <c r="M13" s="48"/>
+      <c r="N13" s="47"/>
       <c r="O13" s="35"/>
       <c r="P13" s="35"/>
       <c r="Q13" s="36"/>
       <c r="R13" s="1"/>
     </row>
-    <row r="14" ht="15.0" customHeight="1">
+    <row r="14" ht="23.25">
       <c r="A14" s="1"/>
-      <c r="B14" s="48" t="s">
+      <c r="B14" s="49" t="s">
         <v>15</v>
       </c>
       <c r="C14" s="24"/>
@@ -1298,49 +1301,49 @@
       <c r="E14" s="24"/>
       <c r="F14" s="24"/>
       <c r="G14" s="25"/>
-      <c r="H14" s="49" t="s">
+      <c r="H14" s="50" t="s">
         <v>16</v>
       </c>
-      <c r="I14" s="45"/>
-      <c r="J14" s="49" t="s">
+      <c r="I14" s="46"/>
+      <c r="J14" s="50" t="s">
         <v>17</v>
       </c>
       <c r="K14" s="19"/>
       <c r="L14" s="19"/>
-      <c r="M14" s="45"/>
-      <c r="N14" s="49" t="s">
+      <c r="M14" s="46"/>
+      <c r="N14" s="50" t="s">
         <v>18</v>
       </c>
       <c r="O14" s="19"/>
       <c r="P14" s="19"/>
-      <c r="Q14" s="45"/>
-      <c r="R14" s="50"/>
-    </row>
-    <row r="15" ht="15.0" customHeight="1">
+      <c r="Q14" s="46"/>
+      <c r="R14" s="51"/>
+    </row>
+    <row r="15">
       <c r="A15" s="1"/>
-      <c r="B15" s="51" t="s">
+      <c r="B15" s="52" t="s">
         <v>19</v>
       </c>
       <c r="C15" s="3"/>
       <c r="D15" s="3"/>
       <c r="E15" s="3"/>
       <c r="F15" s="3"/>
-      <c r="G15" s="52"/>
-      <c r="H15" s="51" t="s">
+      <c r="G15" s="53"/>
+      <c r="H15" s="52" t="s">
         <v>20</v>
       </c>
       <c r="I15" s="3"/>
-      <c r="J15" s="52"/>
-      <c r="K15" s="53" t="s">
+      <c r="J15" s="53"/>
+      <c r="K15" s="54" t="s">
         <v>21</v>
       </c>
-      <c r="L15" s="52"/>
-      <c r="M15" s="54" t="s">
+      <c r="L15" s="53"/>
+      <c r="M15" s="55" t="s">
         <v>22</v>
       </c>
       <c r="N15" s="27"/>
       <c r="O15" s="28"/>
-      <c r="P15" s="55" t="s">
+      <c r="P15" s="56" t="s">
         <v>23</v>
       </c>
       <c r="Q15" s="4"/>
@@ -1348,50 +1351,50 @@
     </row>
     <row r="16">
       <c r="A16" s="1"/>
-      <c r="B16" s="44"/>
+      <c r="B16" s="45"/>
       <c r="C16" s="19"/>
       <c r="D16" s="19"/>
       <c r="E16" s="19"/>
       <c r="F16" s="19"/>
-      <c r="G16" s="56"/>
-      <c r="H16" s="44"/>
+      <c r="G16" s="57"/>
+      <c r="H16" s="45"/>
       <c r="I16" s="19"/>
-      <c r="J16" s="56"/>
-      <c r="K16" s="57"/>
-      <c r="L16" s="56"/>
-      <c r="M16" s="58" t="s">
+      <c r="J16" s="57"/>
+      <c r="K16" s="58"/>
+      <c r="L16" s="57"/>
+      <c r="M16" s="59" t="s">
         <v>24</v>
       </c>
-      <c r="N16" s="59" t="s">
+      <c r="N16" s="60" t="s">
         <v>25</v>
       </c>
-      <c r="O16" s="60"/>
-      <c r="P16" s="57"/>
-      <c r="Q16" s="45"/>
+      <c r="O16" s="61"/>
+      <c r="P16" s="58"/>
+      <c r="Q16" s="46"/>
       <c r="R16" s="1"/>
     </row>
     <row r="17" ht="28.5" customHeight="1">
       <c r="A17" s="1"/>
-      <c r="B17" s="61" t="s">
+      <c r="B17" s="62" t="s">
         <v>26</v>
       </c>
-      <c r="G17" s="62"/>
-      <c r="H17" s="63" t="s">
+      <c r="G17" s="63"/>
+      <c r="H17" s="64" t="s">
         <v>27</v>
       </c>
-      <c r="J17" s="62"/>
-      <c r="K17" s="64" t="s">
+      <c r="J17" s="63"/>
+      <c r="K17" s="65" t="s">
         <v>28</v>
       </c>
-      <c r="L17" s="62"/>
-      <c r="M17" s="65" t="s">
+      <c r="L17" s="63"/>
+      <c r="M17" s="66" t="s">
         <v>29</v>
       </c>
-      <c r="N17" s="64" t="s">
+      <c r="N17" s="65" t="s">
         <v>30</v>
       </c>
-      <c r="O17" s="62"/>
-      <c r="P17" s="64" t="s">
+      <c r="O17" s="63"/>
+      <c r="P17" s="65" t="s">
         <v>31</v>
       </c>
       <c r="Q17" s="9"/>
@@ -1399,27 +1402,27 @@
     </row>
     <row r="18" ht="18.75" customHeight="1">
       <c r="A18" s="1"/>
-      <c r="B18" s="66" t="s">
+      <c r="B18" s="67" t="s">
         <v>23</v>
       </c>
       <c r="C18" s="24"/>
       <c r="D18" s="24"/>
       <c r="E18" s="24"/>
       <c r="F18" s="24"/>
-      <c r="G18" s="67"/>
-      <c r="H18" s="68"/>
+      <c r="G18" s="68"/>
+      <c r="H18" s="69"/>
       <c r="I18" s="24"/>
-      <c r="J18" s="67"/>
-      <c r="K18" s="69" t="s">
+      <c r="J18" s="68"/>
+      <c r="K18" s="70" t="s">
         <v>32</v>
       </c>
-      <c r="L18" s="67"/>
-      <c r="M18" s="70"/>
-      <c r="N18" s="69" t="s">
+      <c r="L18" s="68"/>
+      <c r="M18" s="71"/>
+      <c r="N18" s="70" t="s">
         <v>33</v>
       </c>
-      <c r="O18" s="67"/>
-      <c r="P18" s="69" t="s">
+      <c r="O18" s="68"/>
+      <c r="P18" s="70" t="s">
         <v>34</v>
       </c>
       <c r="Q18" s="25"/>
@@ -1427,7 +1430,7 @@
     </row>
     <row r="19">
       <c r="A19" s="1"/>
-      <c r="B19" s="71" t="s">
+      <c r="B19" s="72" t="s">
         <v>35</v>
       </c>
       <c r="C19" s="19"/>
@@ -1438,14 +1441,14 @@
       <c r="H19" s="19"/>
       <c r="I19" s="19"/>
       <c r="J19" s="19"/>
-      <c r="K19" s="72" t="s">
+      <c r="K19" s="73" t="s">
         <v>36</v>
       </c>
       <c r="L19" s="35"/>
       <c r="M19" s="35"/>
       <c r="N19" s="35"/>
-      <c r="O19" s="47"/>
-      <c r="P19" s="73" t="s">
+      <c r="O19" s="48"/>
+      <c r="P19" s="74" t="s">
         <v>32</v>
       </c>
       <c r="Q19" s="36"/>
@@ -1453,7 +1456,7 @@
     </row>
     <row r="20">
       <c r="A20" s="1"/>
-      <c r="B20" s="74" t="s">
+      <c r="B20" s="75" t="s">
         <v>37</v>
       </c>
       <c r="C20" s="3"/>
@@ -1464,14 +1467,14 @@
       <c r="H20" s="3"/>
       <c r="I20" s="3"/>
       <c r="J20" s="4"/>
-      <c r="K20" s="75" t="s">
+      <c r="K20" s="76" t="s">
         <v>38</v>
       </c>
       <c r="L20" s="40"/>
       <c r="M20" s="40"/>
       <c r="N20" s="40"/>
-      <c r="O20" s="76"/>
-      <c r="P20" s="77" t="s">
+      <c r="O20" s="77"/>
+      <c r="P20" s="78" t="s">
         <v>33</v>
       </c>
       <c r="Q20" s="41"/>
@@ -1479,7 +1482,7 @@
     </row>
     <row r="21">
       <c r="A21" s="1"/>
-      <c r="B21" s="44"/>
+      <c r="B21" s="45"/>
       <c r="C21" s="19"/>
       <c r="D21" s="19"/>
       <c r="E21" s="19"/>
@@ -1487,23 +1490,23 @@
       <c r="G21" s="19"/>
       <c r="H21" s="19"/>
       <c r="I21" s="19"/>
-      <c r="J21" s="45"/>
-      <c r="K21" s="78" t="s">
+      <c r="J21" s="46"/>
+      <c r="K21" s="79" t="s">
         <v>39</v>
       </c>
-      <c r="L21" s="79"/>
-      <c r="M21" s="79"/>
-      <c r="N21" s="79"/>
-      <c r="O21" s="60"/>
-      <c r="P21" s="80" t="s">
+      <c r="L21" s="80"/>
+      <c r="M21" s="80"/>
+      <c r="N21" s="80"/>
+      <c r="O21" s="61"/>
+      <c r="P21" s="81" t="s">
         <v>34</v>
       </c>
-      <c r="Q21" s="81"/>
+      <c r="Q21" s="82"/>
       <c r="R21" s="1"/>
     </row>
     <row r="22">
       <c r="A22" s="1"/>
-      <c r="B22" s="82" t="s">
+      <c r="B22" s="83" t="s">
         <v>40</v>
       </c>
       <c r="C22" s="3"/>
@@ -1511,17 +1514,17 @@
       <c r="E22" s="3"/>
       <c r="F22" s="3"/>
       <c r="G22" s="4"/>
-      <c r="H22" s="83"/>
+      <c r="H22" s="84"/>
       <c r="I22" s="3"/>
       <c r="J22" s="4"/>
-      <c r="K22" s="84" t="s">
+      <c r="K22" s="85" t="s">
         <v>41</v>
       </c>
       <c r="L22" s="24"/>
       <c r="M22" s="24"/>
       <c r="N22" s="24"/>
       <c r="O22" s="25"/>
-      <c r="P22" s="85">
+      <c r="P22" s="86">
         <v>0.0</v>
       </c>
       <c r="Q22" s="25"/>
@@ -1533,7 +1536,7 @@
       <c r="G23" s="9"/>
       <c r="H23" s="10"/>
       <c r="J23" s="9"/>
-      <c r="K23" s="51" t="s">
+      <c r="K23" s="52" t="s">
         <v>42</v>
       </c>
       <c r="L23" s="3"/>
@@ -1560,7 +1563,7 @@
       <c r="G25" s="9"/>
       <c r="H25" s="10"/>
       <c r="J25" s="9"/>
-      <c r="K25" s="83"/>
+      <c r="K25" s="84"/>
       <c r="L25" s="3"/>
       <c r="M25" s="3"/>
       <c r="N25" s="3"/>
@@ -1595,27 +1598,27 @@
       <c r="G28" s="9"/>
       <c r="H28" s="10"/>
       <c r="J28" s="9"/>
-      <c r="K28" s="44"/>
+      <c r="K28" s="45"/>
       <c r="L28" s="19"/>
       <c r="M28" s="19"/>
       <c r="N28" s="19"/>
       <c r="O28" s="19"/>
       <c r="P28" s="19"/>
-      <c r="Q28" s="45"/>
+      <c r="Q28" s="46"/>
       <c r="R28" s="1"/>
     </row>
     <row r="29">
       <c r="A29" s="1"/>
-      <c r="B29" s="44"/>
+      <c r="B29" s="45"/>
       <c r="C29" s="19"/>
       <c r="D29" s="19"/>
       <c r="E29" s="19"/>
       <c r="F29" s="19"/>
-      <c r="G29" s="45"/>
-      <c r="H29" s="44"/>
+      <c r="G29" s="46"/>
+      <c r="H29" s="45"/>
       <c r="I29" s="19"/>
-      <c r="J29" s="45"/>
-      <c r="K29" s="71" t="s">
+      <c r="J29" s="46"/>
+      <c r="K29" s="72" t="s">
         <v>43</v>
       </c>
       <c r="L29" s="19"/>
@@ -1623,7 +1626,7 @@
       <c r="N29" s="19"/>
       <c r="O29" s="19"/>
       <c r="P29" s="19"/>
-      <c r="Q29" s="45"/>
+      <c r="Q29" s="46"/>
       <c r="R29" s="1"/>
     </row>
     <row r="30" ht="3.75" customHeight="1">
@@ -1646,67 +1649,67 @@
       <c r="Q30" s="1"/>
       <c r="R30" s="1"/>
     </row>
-    <row r="31" ht="15.0" customHeight="1">
-      <c r="B31" s="86" t="s">
+    <row r="31">
+      <c r="B31" s="87" t="s">
         <v>44</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="54">
-    <mergeCell ref="B8:Q9"/>
-    <mergeCell ref="B10:K10"/>
-    <mergeCell ref="L10:Q10"/>
-    <mergeCell ref="B7:K7"/>
-    <mergeCell ref="B6:Q6"/>
     <mergeCell ref="H15:J16"/>
+    <mergeCell ref="H17:J17"/>
+    <mergeCell ref="J14:M14"/>
+    <mergeCell ref="K15:L16"/>
+    <mergeCell ref="H14:I14"/>
+    <mergeCell ref="N14:Q14"/>
+    <mergeCell ref="P15:Q16"/>
+    <mergeCell ref="M15:O15"/>
+    <mergeCell ref="N16:O16"/>
+    <mergeCell ref="N17:O17"/>
+    <mergeCell ref="P19:Q19"/>
+    <mergeCell ref="P18:Q18"/>
+    <mergeCell ref="P21:Q21"/>
+    <mergeCell ref="K21:O21"/>
+    <mergeCell ref="K19:O19"/>
+    <mergeCell ref="P17:Q17"/>
+    <mergeCell ref="K20:O20"/>
+    <mergeCell ref="N18:O18"/>
+    <mergeCell ref="K17:L17"/>
+    <mergeCell ref="B12:G13"/>
     <mergeCell ref="B14:G14"/>
     <mergeCell ref="B15:G16"/>
-    <mergeCell ref="J14:M14"/>
-    <mergeCell ref="N14:Q14"/>
-    <mergeCell ref="P15:Q16"/>
-    <mergeCell ref="L7:Q7"/>
-    <mergeCell ref="F3:N3"/>
+    <mergeCell ref="B17:G17"/>
+    <mergeCell ref="B7:K7"/>
     <mergeCell ref="B3:C4"/>
     <mergeCell ref="G4:M4"/>
     <mergeCell ref="O3:Q4"/>
+    <mergeCell ref="G5:M5"/>
+    <mergeCell ref="F3:N3"/>
     <mergeCell ref="B2:Q2"/>
-    <mergeCell ref="G5:M5"/>
+    <mergeCell ref="L11:Q11"/>
+    <mergeCell ref="B11:K11"/>
+    <mergeCell ref="B6:Q6"/>
+    <mergeCell ref="B8:Q9"/>
+    <mergeCell ref="L7:Q7"/>
+    <mergeCell ref="H12:I13"/>
+    <mergeCell ref="L10:Q10"/>
+    <mergeCell ref="B10:K10"/>
+    <mergeCell ref="J12:M13"/>
+    <mergeCell ref="N12:Q13"/>
     <mergeCell ref="K25:Q28"/>
-    <mergeCell ref="B22:G29"/>
-    <mergeCell ref="H22:J29"/>
-    <mergeCell ref="P22:Q22"/>
-    <mergeCell ref="K21:O21"/>
-    <mergeCell ref="K20:O20"/>
-    <mergeCell ref="K22:O22"/>
-    <mergeCell ref="K29:Q29"/>
     <mergeCell ref="K23:Q24"/>
-    <mergeCell ref="B31:Q31"/>
-    <mergeCell ref="P21:Q21"/>
-    <mergeCell ref="B20:J21"/>
     <mergeCell ref="H18:J18"/>
     <mergeCell ref="K18:L18"/>
-    <mergeCell ref="B17:G17"/>
     <mergeCell ref="B18:G18"/>
-    <mergeCell ref="N17:O17"/>
-    <mergeCell ref="K17:L17"/>
-    <mergeCell ref="H17:J17"/>
-    <mergeCell ref="M15:O15"/>
-    <mergeCell ref="N16:O16"/>
-    <mergeCell ref="K15:L16"/>
-    <mergeCell ref="N18:O18"/>
-    <mergeCell ref="H14:I14"/>
-    <mergeCell ref="B12:G13"/>
-    <mergeCell ref="H12:I13"/>
-    <mergeCell ref="J12:M13"/>
-    <mergeCell ref="N12:Q13"/>
-    <mergeCell ref="B11:K11"/>
-    <mergeCell ref="L11:Q11"/>
+    <mergeCell ref="B20:J21"/>
+    <mergeCell ref="B19:J19"/>
     <mergeCell ref="P20:Q20"/>
-    <mergeCell ref="P19:Q19"/>
-    <mergeCell ref="P18:Q18"/>
-    <mergeCell ref="P17:Q17"/>
-    <mergeCell ref="K19:O19"/>
-    <mergeCell ref="B19:J19"/>
+    <mergeCell ref="H22:J29"/>
+    <mergeCell ref="B22:G29"/>
+    <mergeCell ref="K29:Q29"/>
+    <mergeCell ref="B31:Q31"/>
+    <mergeCell ref="K22:O22"/>
+    <mergeCell ref="P22:Q22"/>
   </mergeCells>
   <drawing r:id="rId1"/>
 </worksheet>

</xml_diff>